<commit_message>
Adding Regular Season Data
</commit_message>
<xml_diff>
--- a/Prep_Work/data_sets/2022_data.xlsx
+++ b/Prep_Work/data_sets/2022_data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bryanwenger/Desktop/Desktop_Master/Coding/github_projects/fantasy_football/Prep_Work/data_sets/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3EA4DA3D-AD1F-2D47-B786-6E848EFCEE9B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D749AB9-E19C-9349-A6D6-7250C50452F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16020" xr2:uid="{07630095-4154-FA4F-B841-F42F74202401}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -295,7 +295,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="0.000"/>
+    <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -382,7 +382,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
@@ -706,10 +706,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B34A81C8-9D16-F24C-9E75-E8CD8356D560}">
   <dimension ref="A1:U57"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A26" workbookViewId="0">
       <pane xSplit="1" topLeftCell="H1" activePane="topRight" state="frozen"/>
       <selection activeCell="A28" sqref="A28"/>
-      <selection pane="topRight" activeCell="T1" sqref="T1"/>
+      <selection pane="topRight" activeCell="P60" sqref="P60"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -830,14 +830,16 @@
       <c r="O2" s="3">
         <v>18.100000000000001</v>
       </c>
-      <c r="P2" s="3"/>
+      <c r="P2" s="3">
+        <v>19.48</v>
+      </c>
       <c r="T2">
         <f>SUM(C2:S2)</f>
-        <v>211.42</v>
+        <v>230.89999999999998</v>
       </c>
       <c r="U2" s="9">
         <f>AVERAGE(C2:S2)</f>
-        <v>17.618333333333332</v>
+        <v>17.761538461538461</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.2">
@@ -880,14 +882,16 @@
       <c r="O3" s="3">
         <v>15.1</v>
       </c>
-      <c r="P3" s="3"/>
+      <c r="P3" s="3">
+        <v>15.1</v>
+      </c>
       <c r="T3">
         <f t="shared" ref="T3:T56" si="0">SUM(C3:S3)</f>
-        <v>118.8</v>
+        <v>133.9</v>
       </c>
       <c r="U3" s="9">
         <f t="shared" ref="U3:U57" si="1">AVERAGE(C3:S3)</f>
-        <v>11.879999999999999</v>
+        <v>12.172727272727274</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.2">
@@ -969,14 +973,16 @@
       <c r="O5" s="3">
         <v>15.2</v>
       </c>
-      <c r="P5" s="3"/>
+      <c r="P5" s="3">
+        <v>3.7</v>
+      </c>
       <c r="T5">
         <f t="shared" si="0"/>
-        <v>180.2</v>
+        <v>183.89999999999998</v>
       </c>
       <c r="U5" s="9">
         <f t="shared" si="1"/>
-        <v>15.016666666666666</v>
+        <v>14.146153846153844</v>
       </c>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.2">
@@ -1021,13 +1027,16 @@
       <c r="O6" s="1">
         <v>5.9</v>
       </c>
+      <c r="P6" s="1">
+        <v>5.4</v>
+      </c>
       <c r="T6">
         <f t="shared" si="0"/>
-        <v>95.100000000000009</v>
+        <v>100.50000000000001</v>
       </c>
       <c r="U6" s="9">
         <f t="shared" si="1"/>
-        <v>8.6454545454545464</v>
+        <v>8.3750000000000018</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.2">
@@ -1072,14 +1081,16 @@
       <c r="O7" s="3">
         <v>5.4</v>
       </c>
-      <c r="P7" s="3"/>
+      <c r="P7" s="3">
+        <v>1.7</v>
+      </c>
       <c r="T7">
         <f t="shared" si="0"/>
-        <v>98.2</v>
+        <v>99.9</v>
       </c>
       <c r="U7" s="9">
         <f t="shared" si="1"/>
-        <v>8.9272727272727277</v>
+        <v>8.3250000000000011</v>
       </c>
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.2">
@@ -1220,14 +1231,16 @@
       <c r="O10" s="3">
         <v>5</v>
       </c>
-      <c r="P10" s="3"/>
+      <c r="P10" s="3">
+        <v>7</v>
+      </c>
       <c r="T10">
         <f t="shared" si="0"/>
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="U10" s="9">
         <f t="shared" si="1"/>
-        <v>5.666666666666667</v>
+        <v>5.7692307692307692</v>
       </c>
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.2">
@@ -1711,14 +1724,16 @@
       <c r="O22" s="3">
         <v>5</v>
       </c>
-      <c r="P22" s="3"/>
+      <c r="P22" s="3">
+        <v>0</v>
+      </c>
       <c r="T22">
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="U22" s="9">
         <f t="shared" si="1"/>
-        <v>6.333333333333333</v>
+        <v>4.75</v>
       </c>
     </row>
     <row r="23" spans="1:21" x14ac:dyDescent="0.2">
@@ -1911,13 +1926,16 @@
       <c r="O27" s="3">
         <v>3.6</v>
       </c>
+      <c r="P27" s="1">
+        <v>0</v>
+      </c>
       <c r="T27">
         <f t="shared" si="0"/>
         <v>108.50000000000001</v>
       </c>
       <c r="U27" s="9">
         <f t="shared" si="1"/>
-        <v>15.500000000000002</v>
+        <v>13.562500000000002</v>
       </c>
     </row>
     <row r="28" spans="1:21" x14ac:dyDescent="0.2">
@@ -2000,13 +2018,16 @@
       <c r="O29" s="3">
         <v>5.6</v>
       </c>
+      <c r="P29" s="3">
+        <v>12.7</v>
+      </c>
       <c r="T29">
         <f t="shared" si="0"/>
-        <v>55.8</v>
+        <v>68.5</v>
       </c>
       <c r="U29" s="9">
         <f t="shared" si="1"/>
-        <v>9.2999999999999989</v>
+        <v>9.7857142857142865</v>
       </c>
     </row>
     <row r="30" spans="1:21" x14ac:dyDescent="0.2">
@@ -2251,13 +2272,13 @@
       <c r="M36" s="3">
         <v>22.62</v>
       </c>
-      <c r="N36" s="1"/>
+      <c r="N36" s="1">
+        <v>0</v>
+      </c>
       <c r="O36" s="1">
         <v>19.260000000000002</v>
       </c>
-      <c r="P36" s="1">
-        <v>0</v>
-      </c>
+      <c r="P36" s="1"/>
       <c r="T36">
         <f t="shared" si="0"/>
         <v>123.98</v>
@@ -2295,13 +2316,16 @@
       <c r="O37" s="1">
         <v>11.9</v>
       </c>
+      <c r="P37" s="1">
+        <v>11.4</v>
+      </c>
       <c r="T37">
         <f t="shared" si="0"/>
-        <v>35.5</v>
+        <v>46.9</v>
       </c>
       <c r="U37" s="9">
         <f t="shared" si="1"/>
-        <v>8.875</v>
+        <v>9.379999999999999</v>
       </c>
     </row>
     <row r="38" spans="1:21" x14ac:dyDescent="0.2">
@@ -2471,13 +2495,16 @@
       <c r="O42" s="1">
         <v>12.4</v>
       </c>
+      <c r="P42" s="3">
+        <v>7.7</v>
+      </c>
       <c r="T42">
         <f t="shared" si="0"/>
-        <v>24.3</v>
+        <v>32</v>
       </c>
       <c r="U42" s="9">
         <f t="shared" si="1"/>
-        <v>12.15</v>
+        <v>10.666666666666666</v>
       </c>
     </row>
     <row r="43" spans="1:21" x14ac:dyDescent="0.2">
@@ -2500,13 +2527,16 @@
       <c r="M43" s="11"/>
       <c r="N43" s="11"/>
       <c r="O43" s="1"/>
+      <c r="P43" s="3">
+        <v>6.4</v>
+      </c>
       <c r="T43">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="U43" s="9" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>6.4</v>
+      </c>
+      <c r="U43" s="9">
+        <f t="shared" si="1"/>
+        <v>6.4</v>
       </c>
     </row>
     <row r="44" spans="1:21" x14ac:dyDescent="0.2">
@@ -2564,13 +2594,16 @@
       <c r="M45" s="11"/>
       <c r="N45" s="11"/>
       <c r="O45" s="11"/>
+      <c r="P45" s="1">
+        <v>5.6</v>
+      </c>
       <c r="T45">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="U45" s="9" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>5.6</v>
+      </c>
+      <c r="U45" s="9">
+        <f t="shared" si="1"/>
+        <v>5.6</v>
       </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.2">
@@ -2593,14 +2626,16 @@
       <c r="M46" s="11"/>
       <c r="N46" s="11"/>
       <c r="O46" s="11"/>
-      <c r="P46" s="3"/>
+      <c r="P46" s="3">
+        <v>14.5</v>
+      </c>
       <c r="T46">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="U46" s="9" t="e">
-        <f t="shared" si="1"/>
-        <v>#DIV/0!</v>
+        <v>14.5</v>
+      </c>
+      <c r="U46" s="9">
+        <f t="shared" si="1"/>
+        <v>14.5</v>
       </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.2">
@@ -2659,13 +2694,17 @@
         <f>O2+O3+O5+O7+O10</f>
         <v>58.800000000000004</v>
       </c>
+      <c r="P47">
+        <f>P2+P3+P5+P7+P10</f>
+        <v>46.980000000000004</v>
+      </c>
       <c r="T47">
         <f t="shared" si="0"/>
-        <v>903.2</v>
+        <v>950.18000000000006</v>
       </c>
       <c r="U47" s="9">
         <f t="shared" si="1"/>
-        <v>69.476923076923086</v>
+        <v>67.87</v>
       </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.2">
@@ -2720,13 +2759,17 @@
         <f>O22+O27+O28+O29+O40</f>
         <v>47.6</v>
       </c>
+      <c r="P48">
+        <f>P22+P29+P42+P43+P46</f>
+        <v>41.3</v>
+      </c>
       <c r="T48">
         <f t="shared" si="0"/>
-        <v>514.72</v>
+        <v>556.02</v>
       </c>
       <c r="U48" s="9">
         <f t="shared" si="1"/>
-        <v>39.593846153846158</v>
+        <v>39.715714285714284</v>
       </c>
     </row>
     <row r="49" spans="1:21" x14ac:dyDescent="0.2">
@@ -2785,9 +2828,9 @@
         <f t="shared" si="2"/>
         <v>0.55263157894736847</v>
       </c>
-      <c r="P49" s="9" t="e">
+      <c r="P49" s="9">
         <f t="shared" si="2"/>
-        <v>#DIV/0!</v>
+        <v>0.5321703670140463</v>
       </c>
       <c r="Q49" s="9" t="e">
         <f t="shared" si="2"/>
@@ -2803,7 +2846,7 @@
       </c>
       <c r="T49" s="9">
         <f t="shared" si="2"/>
-        <v>0.63698939291356349</v>
+        <v>0.63084583720621434</v>
       </c>
       <c r="U49" s="9"/>
     </row>
@@ -2863,9 +2906,9 @@
         <f t="shared" si="3"/>
         <v>0.44736842105263158</v>
       </c>
-      <c r="P50" s="9" t="e">
+      <c r="P50" s="9">
         <f t="shared" si="3"/>
-        <v>#DIV/0!</v>
+        <v>0.46782963298595376</v>
       </c>
       <c r="Q50" s="9" t="e">
         <f t="shared" si="3"/>
@@ -2881,7 +2924,7 @@
       </c>
       <c r="T50" s="9">
         <f t="shared" si="3"/>
-        <v>0.36301060708643645</v>
+        <v>0.36915416279378566</v>
       </c>
       <c r="U50" s="9"/>
     </row>
@@ -2941,13 +2984,17 @@
         <f t="shared" si="4"/>
         <v>106.4</v>
       </c>
+      <c r="P51">
+        <f>P47+P48</f>
+        <v>88.28</v>
+      </c>
       <c r="T51">
         <f t="shared" si="0"/>
-        <v>1417.92</v>
+        <v>1506.2</v>
       </c>
       <c r="U51" s="9">
         <f t="shared" si="1"/>
-        <v>109.07076923076923</v>
+        <v>107.58571428571429</v>
       </c>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.2">
@@ -2993,13 +3040,16 @@
       <c r="O52">
         <v>103.8</v>
       </c>
+      <c r="P52">
+        <v>96.5</v>
+      </c>
       <c r="T52">
         <f t="shared" si="0"/>
-        <v>1347</v>
+        <v>1443.5</v>
       </c>
       <c r="U52" s="9">
         <f t="shared" si="1"/>
-        <v>103.61538461538461</v>
+        <v>103.10714285714286</v>
       </c>
     </row>
     <row r="53" spans="1:21" x14ac:dyDescent="0.2">
@@ -3011,7 +3061,7 @@
         <v>11.959999999999994</v>
       </c>
       <c r="D53">
-        <f t="shared" ref="D53:T54" si="5">D51-D52</f>
+        <f t="shared" ref="D53:T53" si="5">D51-D52</f>
         <v>36.260000000000005</v>
       </c>
       <c r="E53">
@@ -3060,7 +3110,7 @@
       </c>
       <c r="P53">
         <f t="shared" si="5"/>
-        <v>0</v>
+        <v>-8.2199999999999989</v>
       </c>
       <c r="Q53">
         <f t="shared" si="5"/>
@@ -3076,11 +3126,11 @@
       </c>
       <c r="T53">
         <f t="shared" si="5"/>
-        <v>70.920000000000073</v>
+        <v>62.700000000000045</v>
       </c>
       <c r="U53" s="9">
         <f t="shared" si="1"/>
-        <v>4.1717647058823522</v>
+        <v>3.6882352941176464</v>
       </c>
     </row>
     <row r="54" spans="1:21" x14ac:dyDescent="0.2">
@@ -3126,13 +3176,16 @@
       <c r="O54">
         <v>1</v>
       </c>
+      <c r="P54">
+        <v>0</v>
+      </c>
       <c r="T54">
         <f>SUM(B54:S54)</f>
         <v>9</v>
       </c>
       <c r="U54" s="8">
         <f t="shared" si="1"/>
-        <v>0.69230769230769229</v>
+        <v>0.6428571428571429</v>
       </c>
     </row>
     <row r="55" spans="1:21" x14ac:dyDescent="0.2">
@@ -3190,13 +3243,17 @@
         <f>O36+O42+O3+O5+O7+O10+O22+O28+O40+O37</f>
         <v>122.66000000000003</v>
       </c>
+      <c r="P55">
+        <f>P46+P43+P42+P37+P29+P22+P10+P7+P3+P2</f>
+        <v>95.98</v>
+      </c>
       <c r="T55">
         <f t="shared" si="0"/>
-        <v>1585.88</v>
+        <v>1681.8600000000001</v>
       </c>
       <c r="U55" s="9">
         <f t="shared" si="1"/>
-        <v>121.99076923076925</v>
+        <v>120.13285714285715</v>
       </c>
     </row>
     <row r="56" spans="1:21" x14ac:dyDescent="0.2">
@@ -3255,13 +3312,17 @@
         <f t="shared" si="6"/>
         <v>-16.260000000000019</v>
       </c>
+      <c r="P56">
+        <f>P51-P55</f>
+        <v>-7.7000000000000028</v>
+      </c>
       <c r="T56">
         <f t="shared" si="0"/>
-        <v>-167.96</v>
+        <v>-175.66000000000003</v>
       </c>
       <c r="U56" s="9">
         <f t="shared" si="1"/>
-        <v>-12.92</v>
+        <v>-12.547142857142859</v>
       </c>
     </row>
     <row r="57" spans="1:21" x14ac:dyDescent="0.2">
@@ -3273,7 +3334,7 @@
         <v>0.87350974120383829</v>
       </c>
       <c r="D57" s="10">
-        <f t="shared" ref="D57:O57" si="7">D51/D55</f>
+        <f t="shared" ref="D57:P57" si="7">D51/D55</f>
         <v>0.91443018280824584</v>
       </c>
       <c r="E57" s="10">
@@ -3320,17 +3381,20 @@
         <f t="shared" si="7"/>
         <v>0.86743844774172496</v>
       </c>
-      <c r="P57" s="9"/>
+      <c r="P57" s="10">
+        <f t="shared" si="7"/>
+        <v>0.91977495311523227</v>
+      </c>
       <c r="Q57" s="9"/>
       <c r="R57" s="9"/>
       <c r="S57" s="9"/>
       <c r="T57" s="9">
         <f>SUM(C57:S57)</f>
-        <v>11.706105173487044</v>
+        <v>12.625880126602276</v>
       </c>
       <c r="U57" s="9">
         <f t="shared" si="1"/>
-        <v>0.90046962872977265</v>
+        <v>0.90184858047159111</v>
       </c>
     </row>
   </sheetData>

</xml_diff>